<commit_message>
Fix column mapping failing due to asterisk in column names; Default column data type to string when reading excel to preserve leading zeroes for bank acc
</commit_message>
<xml_diff>
--- a/data/sample_data/Employee.xlsx
+++ b/data/sample_data/Employee.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Employee</t>
   </si>
@@ -150,6 +150,9 @@
     </r>
   </si>
   <si>
+    <t>00080230135</t>
+  </si>
+  <si>
     <t>SGD</t>
   </si>
   <si>
@@ -188,6 +191,9 @@
     </r>
   </si>
   <si>
+    <t>00528270302</t>
+  </si>
+  <si>
     <t>xadkins067</t>
   </si>
   <si>
@@ -226,6 +232,9 @@
     </r>
   </si>
   <si>
+    <t>00098876895</t>
+  </si>
+  <si>
     <t>mhiggs048</t>
   </si>
 </sst>
@@ -236,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -246,6 +255,11 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
@@ -260,7 +274,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,8 +293,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -292,6 +312,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -305,7 +347,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -314,7 +356,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -323,13 +365,88 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -337,57 +454,84 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -399,47 +543,80 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -459,8 +636,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -479,10 +658,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -659,11 +838,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -672,34 +854,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -947,12 +1129,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1243,7 +1425,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1524,7 +1706,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AF5"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1568,339 +1750,509 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="M2" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="N2" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="O2" t="s" s="3">
+      <c r="O2" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="P2" t="s" s="3">
+      <c r="P2" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="Q2" t="s" s="3">
+      <c r="Q2" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="R2" t="s" s="3">
+      <c r="R2" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="S2" t="s" s="3">
+      <c r="S2" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="T2" t="s" s="3">
+      <c r="T2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="U2" t="s" s="3">
+      <c r="U2" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="V2" t="s" s="3">
+      <c r="V2" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="W2" t="s" s="3">
+      <c r="W2" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="X2" t="s" s="3">
+      <c r="X2" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="Y2" t="s" s="3">
+      <c r="Y2" t="s" s="5">
         <v>25</v>
       </c>
-      <c r="Z2" t="s" s="3">
+      <c r="Z2" t="s" s="5">
         <v>26</v>
       </c>
-      <c r="AA2" t="s" s="3">
+      <c r="AA2" t="s" s="5">
         <v>27</v>
       </c>
-      <c r="AB2" t="s" s="3">
+      <c r="AB2" t="s" s="5">
         <v>28</v>
       </c>
-      <c r="AC2" t="s" s="3">
+      <c r="AC2" t="s" s="5">
         <v>29</v>
       </c>
-      <c r="AD2" t="s" s="3">
+      <c r="AD2" t="s" s="5">
         <v>30</v>
       </c>
-      <c r="AE2" t="s" s="3">
+      <c r="AE2" t="s" s="5">
         <v>31</v>
       </c>
-      <c r="AF2" t="s" s="3">
+      <c r="AF2" t="s" s="5">
         <v>32</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>11111111</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="7">
         <v>33</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" t="s" s="8">
         <v>34</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" t="s" s="6">
+      <c r="D3" s="9"/>
+      <c r="E3" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" t="s" s="6">
+      <c r="F3" s="9"/>
+      <c r="G3" t="s" s="8">
         <v>36</v>
       </c>
-      <c r="H3" t="s" s="6">
+      <c r="H3" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="I3" t="s" s="6">
+      <c r="I3" t="s" s="8">
         <v>38</v>
       </c>
-      <c r="J3" t="s" s="6">
+      <c r="J3" t="s" s="8">
         <v>39</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" t="s" s="6">
+      <c r="K3" s="9"/>
+      <c r="L3" t="s" s="8">
         <v>40</v>
       </c>
-      <c r="M3" t="s" s="6">
+      <c r="M3" t="s" s="8">
         <v>41</v>
       </c>
-      <c r="N3" t="s" s="6">
+      <c r="N3" t="s" s="8">
         <v>36</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" t="s" s="6">
+      <c r="O3" s="9"/>
+      <c r="P3" t="s" s="8">
         <v>42</v>
       </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="8">
-        <v>80230135</v>
-      </c>
-      <c r="Z3" s="8">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="Z3" s="10">
         <v>81</v>
       </c>
-      <c r="AA3" s="8">
+      <c r="AA3" s="10">
         <v>7171</v>
       </c>
-      <c r="AB3" t="s" s="6">
-        <v>43</v>
-      </c>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" t="s" s="6">
+      <c r="AB3" t="s" s="8">
         <v>44</v>
+      </c>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" t="s" s="8">
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="9">
+      <c r="A4" s="11">
         <v>11111112</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s" s="11">
+      <c r="B4" t="s" s="12">
         <v>46</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" t="s" s="11">
+      <c r="C4" t="s" s="13">
         <v>47</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" t="s" s="11">
+      <c r="D4" s="14"/>
+      <c r="E4" t="s" s="13">
         <v>48</v>
       </c>
-      <c r="H4" t="s" s="11">
+      <c r="F4" s="14"/>
+      <c r="G4" t="s" s="13">
         <v>49</v>
       </c>
-      <c r="I4" t="s" s="11">
+      <c r="H4" t="s" s="13">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s" s="13">
         <v>38</v>
       </c>
-      <c r="J4" t="s" s="11">
-        <v>50</v>
-      </c>
-      <c r="K4" s="12"/>
-      <c r="L4" t="s" s="11">
+      <c r="J4" t="s" s="13">
+        <v>51</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" t="s" s="13">
         <v>40</v>
       </c>
-      <c r="M4" t="s" s="11">
+      <c r="M4" t="s" s="13">
         <v>41</v>
       </c>
-      <c r="N4" t="s" s="11">
-        <v>51</v>
-      </c>
-      <c r="O4" s="12"/>
-      <c r="P4" t="s" s="11">
+      <c r="N4" t="s" s="13">
         <v>52</v>
       </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="13">
-        <v>528270302</v>
-      </c>
-      <c r="Z4" s="13">
+      <c r="O4" s="14"/>
+      <c r="P4" t="s" s="13">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" t="s" s="13">
+        <v>54</v>
+      </c>
+      <c r="Z4" s="15">
         <v>281</v>
       </c>
-      <c r="AA4" s="13">
+      <c r="AA4" s="15">
         <v>7171</v>
       </c>
-      <c r="AB4" t="s" s="11">
-        <v>43</v>
-      </c>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" t="s" s="11">
-        <v>53</v>
+      <c r="AB4" t="s" s="13">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" t="s" s="13">
+        <v>55</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="9">
+      <c r="A5" s="11">
         <v>11111113</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>55</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" t="s" s="11">
+      <c r="B5" t="s" s="12">
         <v>56</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" t="s" s="11">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s" s="11">
+      <c r="C5" t="s" s="13">
         <v>57</v>
       </c>
-      <c r="I5" t="s" s="11">
+      <c r="D5" s="14"/>
+      <c r="E5" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="J5" t="s" s="11">
+      <c r="F5" s="14"/>
+      <c r="G5" t="s" s="13">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s" s="13">
         <v>59</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" t="s" s="11">
+      <c r="I5" t="s" s="13">
         <v>60</v>
       </c>
-      <c r="M5" t="s" s="11">
+      <c r="J5" t="s" s="13">
         <v>61</v>
       </c>
-      <c r="N5" t="s" s="11">
-        <v>51</v>
-      </c>
-      <c r="O5" s="12"/>
-      <c r="P5" t="s" s="11">
+      <c r="K5" s="14"/>
+      <c r="L5" t="s" s="13">
         <v>62</v>
       </c>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="13">
-        <v>98876895</v>
-      </c>
-      <c r="Z5" s="13">
+      <c r="M5" t="s" s="13">
+        <v>63</v>
+      </c>
+      <c r="N5" t="s" s="13">
+        <v>52</v>
+      </c>
+      <c r="O5" s="14"/>
+      <c r="P5" t="s" s="13">
+        <v>64</v>
+      </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" t="s" s="13">
+        <v>65</v>
+      </c>
+      <c r="Z5" s="15">
         <v>18</v>
       </c>
-      <c r="AA5" s="13">
+      <c r="AA5" s="15">
         <v>7171</v>
       </c>
-      <c r="AB5" t="s" s="11">
-        <v>43</v>
-      </c>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" t="s" s="11">
-        <v>63</v>
-      </c>
+      <c r="AB5" t="s" s="13">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" t="s" s="13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="18"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="21"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="21"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="21"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="23"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>